<commit_message>
Added new information about best prepaid card
</commit_message>
<xml_diff>
--- a/Dokumentace/Dokumentační podklady/Operátoři a ceny SIM/Ceny předplacených karet.xlsx
+++ b/Dokumentace/Dokumentační podklady/Operátoři a ceny SIM/Ceny předplacených karet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="41">
   <si>
     <t>Společnost</t>
   </si>
@@ -658,8 +658,8 @@
   </sheetPr>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,7 +1044,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>28</v>
       </c>
@@ -1064,8 +1064,11 @@
       <c r="F17" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
@@ -1086,7 +1089,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
@@ -1107,7 +1110,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
@@ -1128,7 +1131,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
@@ -1149,7 +1152,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
@@ -1170,7 +1173,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>32</v>
       </c>
@@ -1191,7 +1194,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
@@ -1212,7 +1215,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>36</v>
       </c>
@@ -1233,7 +1236,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>36</v>
       </c>
@@ -1254,7 +1257,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>36</v>
       </c>
@@ -1275,7 +1278,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
@@ -1296,7 +1299,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
@@ -1317,7 +1320,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>38</v>
       </c>
@@ -1338,7 +1341,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
@@ -1359,7 +1362,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Updated card prices list
</commit_message>
<xml_diff>
--- a/Dokumentace/Dokumentační podklady/Operátoři a ceny SIM/Ceny předplacených karet.xlsx
+++ b/Dokumentace/Dokumentační podklady/Operátoři a ceny SIM/Ceny předplacených karet.xlsx
@@ -186,7 +186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,6 +196,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -213,7 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -261,6 +267,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -363,6 +375,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9900"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -659,7 +676,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,10 +739,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="14">
@@ -1045,10 +1062,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="18" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="14">

</xml_diff>

<commit_message>
Added informatinou about new SIM provider
</commit_message>
<xml_diff>
--- a/Dokumentace/Dokumentační podklady/Operátoři a ceny SIM/Ceny předplacených karet.xlsx
+++ b/Dokumentace/Dokumentační podklady/Operátoři a ceny SIM/Ceny předplacených karet.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6060"/>
   </bookViews>
   <sheets>
-    <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ceny předplacených karet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="45">
   <si>
     <t>Společnost</t>
   </si>
@@ -147,6 +147,18 @@
   </si>
   <si>
     <t>1 MB</t>
+  </si>
+  <si>
+    <t>Ha-loo mobile</t>
+  </si>
+  <si>
+    <t>Data pro tablet</t>
+  </si>
+  <si>
+    <t>1 kB</t>
+  </si>
+  <si>
+    <t>Data pro mobil</t>
   </si>
 </sst>
 </file>
@@ -301,6 +313,46 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="166" formatCode="#,##0&quot; MB&quot;"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -352,46 +404,6 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -412,16 +424,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabulka1" displayName="Tabulka1" ref="A1:G34" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabulka1" displayName="Tabulka1" ref="A1:G44" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:G44"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Společnost" dataDxfId="6"/>
-    <tableColumn id="2" name="Název produktu" dataDxfId="5"/>
-    <tableColumn id="3" name="Počet dat" dataDxfId="4"/>
-    <tableColumn id="4" name="Cena za 1 MB" dataDxfId="3"/>
-    <tableColumn id="5" name="Cena" dataDxfId="2"/>
-    <tableColumn id="6" name="Mesíčně" dataDxfId="1"/>
-    <tableColumn id="7" name="Nejmenší jednotka" dataDxfId="0"/>
+    <tableColumn id="1" name="Společnost" dataDxfId="10"/>
+    <tableColumn id="2" name="Název produktu" dataDxfId="9"/>
+    <tableColumn id="3" name="Počet dat" dataDxfId="8"/>
+    <tableColumn id="4" name="Cena za 1 MB" dataDxfId="7"/>
+    <tableColumn id="5" name="Cena" dataDxfId="6"/>
+    <tableColumn id="6" name="Mesíčně" dataDxfId="5"/>
+    <tableColumn id="7" name="Nejmenší jednotka" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -695,8 +707,8 @@
   </sheetPr>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,7 +1128,7 @@
         <v>500</v>
       </c>
       <c r="D18" s="3">
-        <f t="shared" ref="D18:D34" si="3">E18/C18</f>
+        <f t="shared" ref="D18:D44" si="3">E18/C18</f>
         <v>0.2</v>
       </c>
       <c r="E18" s="4">
@@ -1420,7 +1432,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>39</v>
       </c>
@@ -1441,7 +1453,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
@@ -1462,43 +1474,256 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D36" s="15"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D37" s="15"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D38" s="15"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D39" s="15"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D40" s="15"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D41" s="15"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D42" s="15"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D43" s="15"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D44" s="15"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="13">
+        <v>3000</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="3"/>
+        <v>0.14666666666666667</v>
+      </c>
+      <c r="E35" s="4">
+        <v>440</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="13">
+        <v>10000</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="3"/>
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="E36" s="4">
+        <v>640</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="13">
+        <v>50</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="3"/>
+        <v>0.7</v>
+      </c>
+      <c r="E37" s="4">
+        <v>35</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="13">
+        <v>100</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+      <c r="E38" s="4">
+        <v>60</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="13">
+        <v>150</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="3"/>
+        <v>0.46</v>
+      </c>
+      <c r="E39" s="4">
+        <v>69</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="13">
+        <v>200</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="3"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E40" s="4">
+        <v>110</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="13">
+        <v>300</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="3"/>
+        <v>0.43</v>
+      </c>
+      <c r="E41" s="4">
+        <v>129</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="13">
+        <v>600</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="3"/>
+        <v>0.33166666666666667</v>
+      </c>
+      <c r="E42" s="4">
+        <v>199</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="13">
+        <v>1200</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="3"/>
+        <v>0.24083333333333334</v>
+      </c>
+      <c r="E43" s="4">
+        <v>289</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G43" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" s="13">
+        <v>1500</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="3"/>
+        <v>0.23266666666666666</v>
+      </c>
+      <c r="E44" s="4">
+        <v>349</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D45" s="15"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D46" s="15"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D47" s="15"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D48" s="15"/>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
@@ -1506,22 +1731,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="NE">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="NE">
       <formula>NOT(ISERROR(SEARCH("NE",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>MIN($D:$D)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>MIN($E:$E)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"NE"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1553,11 +1778,16 @@
     <hyperlink ref="B31" r:id="rId25" location="a_nabidkaPredplaceneKarty"/>
     <hyperlink ref="B32" r:id="rId26"/>
     <hyperlink ref="B33:B34" r:id="rId27" display="Tesco mobile"/>
+    <hyperlink ref="B35" r:id="rId28"/>
+    <hyperlink ref="B36" r:id="rId29"/>
+    <hyperlink ref="B37" r:id="rId30"/>
+    <hyperlink ref="B38:B43" r:id="rId31" display="Data pro mobil"/>
+    <hyperlink ref="B43:B44" r:id="rId32" display="Data pro mobil"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId28"/>
+  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId33"/>
   <tableParts count="1">
-    <tablePart r:id="rId29"/>
+    <tablePart r:id="rId34"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>